<commit_message>
setup excel for SOTA DuC
</commit_message>
<xml_diff>
--- a/sota/src/data.xlsx
+++ b/sota/src/data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ludovic/Documents/thesis/sota/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D53801-B8CD-324D-9916-39BA37885CF5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB826B2-06A2-934F-91B9-659D2502B011}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-10340" windowWidth="51200" windowHeight="28340" xr2:uid="{A557A50A-5DDC-A947-B4B9-80A2CEF9B354}"/>
+    <workbookView xWindow="28800" yWindow="-10340" windowWidth="51200" windowHeight="28340" activeTab="2" xr2:uid="{A557A50A-5DDC-A947-B4B9-80A2CEF9B354}"/>
   </bookViews>
   <sheets>
     <sheet name="DelayedActions" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="ProgressDA" sheetId="3" r:id="rId2"/>
     <sheet name="Uncertainty" sheetId="2" r:id="rId3"/>
+    <sheet name="ProgressDuC" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1301" uniqueCount="758">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1342" uniqueCount="758">
   <si>
     <t>Author</t>
   </si>
@@ -2359,7 +2360,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2406,133 +2407,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Per cent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="76">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="29">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2695,46 +2579,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -2850,316 +2694,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3485,11 +3019,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99048B8C-98B5-C846-BA1E-677FE6633279}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="R187" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="U205" sqref="U205"/>
+      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3511,27 +3045,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="N1" s="17" t="s">
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="N1" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="U1" s="17" t="s">
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="U1" s="18" t="s">
         <v>198</v>
       </c>
-      <c r="V1" s="17"/>
-      <c r="W1" s="17"/>
-      <c r="Y1" s="17" t="s">
+      <c r="V1" s="18"/>
+      <c r="W1" s="18"/>
+      <c r="Y1" s="18" t="s">
         <v>205</v>
       </c>
-      <c r="Z1" s="17"/>
+      <c r="Z1" s="18"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -23319,77 +22853,77 @@
     <mergeCell ref="Y1:Z1"/>
   </mergeCells>
   <conditionalFormatting sqref="Y1:Z1048576">
-    <cfRule type="cellIs" dxfId="29" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="17" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T3:T204">
-    <cfRule type="cellIs" dxfId="28" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="16" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3:S204">
-    <cfRule type="cellIs" dxfId="27" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="15" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:L204">
-    <cfRule type="cellIs" dxfId="26" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="14" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N37:R37">
-    <cfRule type="cellIs" dxfId="25" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="13" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J37:L37">
-    <cfRule type="cellIs" dxfId="24" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="12" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N40:R40">
-    <cfRule type="cellIs" dxfId="23" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="11" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J40:L40">
-    <cfRule type="cellIs" dxfId="22" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="10" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N43:R43">
-    <cfRule type="cellIs" dxfId="21" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="9" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J43:L43">
-    <cfRule type="cellIs" dxfId="20" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="8" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N44:R44">
-    <cfRule type="cellIs" dxfId="19" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="7" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J44:L44">
-    <cfRule type="cellIs" dxfId="18" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="6" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N46:R46">
-    <cfRule type="cellIs" dxfId="17" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J46:L46">
-    <cfRule type="cellIs" dxfId="16" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="4" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:D204">
-    <cfRule type="expression" dxfId="15" priority="1">
+    <cfRule type="expression" dxfId="14" priority="1">
       <formula>SUMPRODUCT(--EXACT($D$3:$D$204,$D3))&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23593,7 +23127,7 @@
   <dimension ref="B3:E11"/>
   <sheetViews>
     <sheetView zoomScale="400" zoomScaleNormal="400" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23689,7 +23223,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D5 D10:D11">
-    <cfRule type="expression" dxfId="75" priority="1">
+    <cfRule type="expression" dxfId="13" priority="1">
       <formula>NOT(AND($D$5=$D$10,$D$5=$D$11))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23699,12 +23233,2527 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C7501BA-1B5B-254E-92CB-F30CCA26173E}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:Z245"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="11.1640625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="0" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="0" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1" s="17"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="V1" s="18"/>
+      <c r="W1" s="18"/>
+      <c r="X1" s="17"/>
+      <c r="Y1" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="Z1" s="18"/>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A2" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="N2" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="O2" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q2" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="R2" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="S2" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="T2" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="U2" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="V2" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="W2" s="17" t="s">
+        <v>228</v>
+      </c>
+      <c r="X2" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y2" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="Z2" s="17" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="str">
+        <f>TRIM(LOWER(C3))</f>
+        <v/>
+      </c>
+      <c r="I3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" t="b">
+        <v>1</v>
+      </c>
+      <c r="K3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L3" t="b">
+        <v>1</v>
+      </c>
+      <c r="M3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N3" t="b">
+        <v>0</v>
+      </c>
+      <c r="O3" t="b">
+        <v>0</v>
+      </c>
+      <c r="T3" t="b">
+        <f>AND(AND(I3:L3),NOT(OR(M3:R3)),NOT(S3))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" ref="D4:D43" si="0">TRIM(LOWER(C4))</f>
+        <v/>
+      </c>
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
+      <c r="M4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I5" t="b">
+        <v>1</v>
+      </c>
+      <c r="M5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I6" t="b">
+        <v>1</v>
+      </c>
+      <c r="M6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I7" t="b">
+        <v>1</v>
+      </c>
+      <c r="M7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I8" t="b">
+        <v>1</v>
+      </c>
+      <c r="M8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I9" t="b">
+        <v>1</v>
+      </c>
+      <c r="M9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I10" t="b">
+        <v>1</v>
+      </c>
+      <c r="M10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I11" t="b">
+        <v>1</v>
+      </c>
+      <c r="M11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I12" t="b">
+        <v>1</v>
+      </c>
+      <c r="M12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I13" t="b">
+        <v>1</v>
+      </c>
+      <c r="M13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I14" t="b">
+        <v>1</v>
+      </c>
+      <c r="M14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I15" t="b">
+        <v>1</v>
+      </c>
+      <c r="M15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I16" t="b">
+        <v>1</v>
+      </c>
+      <c r="M16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I17" t="b">
+        <v>1</v>
+      </c>
+      <c r="M17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I18" t="b">
+        <v>1</v>
+      </c>
+      <c r="M18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I19" t="b">
+        <v>1</v>
+      </c>
+      <c r="M19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I20" t="b">
+        <v>1</v>
+      </c>
+      <c r="M20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I21" t="b">
+        <v>1</v>
+      </c>
+      <c r="M21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I22" t="b">
+        <v>1</v>
+      </c>
+      <c r="M22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I23" t="b">
+        <v>1</v>
+      </c>
+      <c r="M23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I24" t="b">
+        <v>1</v>
+      </c>
+      <c r="M24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I25" t="b">
+        <v>1</v>
+      </c>
+      <c r="M25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I26" t="b">
+        <v>1</v>
+      </c>
+      <c r="M26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I27" t="b">
+        <v>1</v>
+      </c>
+      <c r="M27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I28" t="b">
+        <v>1</v>
+      </c>
+      <c r="M28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I29" t="b">
+        <v>1</v>
+      </c>
+      <c r="M29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I30" t="b">
+        <v>1</v>
+      </c>
+      <c r="M30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I31" t="b">
+        <v>1</v>
+      </c>
+      <c r="M31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I32" t="b">
+        <v>1</v>
+      </c>
+      <c r="M32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I33" t="b">
+        <v>1</v>
+      </c>
+      <c r="M33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I34" t="b">
+        <v>1</v>
+      </c>
+      <c r="M34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I35" t="b">
+        <v>1</v>
+      </c>
+      <c r="M35" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I36" t="b">
+        <v>1</v>
+      </c>
+      <c r="M36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I37" t="b">
+        <v>1</v>
+      </c>
+      <c r="M37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I38" t="b">
+        <v>1</v>
+      </c>
+      <c r="M38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I39" t="b">
+        <v>1</v>
+      </c>
+      <c r="M39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I40" t="b">
+        <v>1</v>
+      </c>
+      <c r="M40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I41" t="b">
+        <v>1</v>
+      </c>
+      <c r="M41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I42" t="b">
+        <v>1</v>
+      </c>
+      <c r="M42" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I43" t="b">
+        <v>1</v>
+      </c>
+      <c r="M43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I44" t="b">
+        <v>1</v>
+      </c>
+      <c r="M44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I45" t="b">
+        <v>1</v>
+      </c>
+      <c r="M45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I46" t="b">
+        <v>1</v>
+      </c>
+      <c r="M46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I47" t="b">
+        <v>1</v>
+      </c>
+      <c r="M47" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="I48" t="b">
+        <v>1</v>
+      </c>
+      <c r="M48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I49" t="b">
+        <v>1</v>
+      </c>
+      <c r="M49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I50" t="b">
+        <v>1</v>
+      </c>
+      <c r="M50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I51" t="b">
+        <v>1</v>
+      </c>
+      <c r="M51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I52" t="b">
+        <v>1</v>
+      </c>
+      <c r="M52" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I53" t="b">
+        <v>1</v>
+      </c>
+      <c r="M53" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I54" t="b">
+        <v>1</v>
+      </c>
+      <c r="M54" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I55" t="b">
+        <v>1</v>
+      </c>
+      <c r="M55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I56" t="b">
+        <v>1</v>
+      </c>
+      <c r="M56" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I57" t="b">
+        <v>1</v>
+      </c>
+      <c r="M57" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I58" t="b">
+        <v>1</v>
+      </c>
+      <c r="M58" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I59" t="b">
+        <v>1</v>
+      </c>
+      <c r="M59" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I60" t="b">
+        <v>1</v>
+      </c>
+      <c r="M60" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I61" t="b">
+        <v>1</v>
+      </c>
+      <c r="M61" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I62" t="b">
+        <v>1</v>
+      </c>
+      <c r="M62" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I63" t="b">
+        <v>1</v>
+      </c>
+      <c r="M63" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I64" t="b">
+        <v>1</v>
+      </c>
+      <c r="M64" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I65" t="b">
+        <v>1</v>
+      </c>
+      <c r="M65" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I66" t="b">
+        <v>1</v>
+      </c>
+      <c r="M66" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I67" t="b">
+        <v>1</v>
+      </c>
+      <c r="M67" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I68" t="b">
+        <v>1</v>
+      </c>
+      <c r="M68" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I69" t="b">
+        <v>1</v>
+      </c>
+      <c r="M69" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I70" t="b">
+        <v>1</v>
+      </c>
+      <c r="M70" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I71" t="b">
+        <v>1</v>
+      </c>
+      <c r="M71" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I72" t="b">
+        <v>1</v>
+      </c>
+      <c r="M72" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I73" t="b">
+        <v>1</v>
+      </c>
+      <c r="M73" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I74" t="b">
+        <v>1</v>
+      </c>
+      <c r="M74" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I75" t="b">
+        <v>1</v>
+      </c>
+      <c r="M75" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I76" t="b">
+        <v>1</v>
+      </c>
+      <c r="M76" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I77" t="b">
+        <v>1</v>
+      </c>
+      <c r="M77" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I78" t="b">
+        <v>1</v>
+      </c>
+      <c r="M78" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I79" t="b">
+        <v>1</v>
+      </c>
+      <c r="M79" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I80" t="b">
+        <v>1</v>
+      </c>
+      <c r="M80" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I81" t="b">
+        <v>1</v>
+      </c>
+      <c r="M81" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I82" t="b">
+        <v>1</v>
+      </c>
+      <c r="M82" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I83" t="b">
+        <v>1</v>
+      </c>
+      <c r="M83" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I84" t="b">
+        <v>1</v>
+      </c>
+      <c r="M84" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I85" t="b">
+        <v>1</v>
+      </c>
+      <c r="M85" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I86" t="b">
+        <v>1</v>
+      </c>
+      <c r="M86" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I87" t="b">
+        <v>1</v>
+      </c>
+      <c r="M87" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I88" t="b">
+        <v>1</v>
+      </c>
+      <c r="M88" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I89" t="b">
+        <v>1</v>
+      </c>
+      <c r="M89" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I90" t="b">
+        <v>1</v>
+      </c>
+      <c r="M90" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I91" t="b">
+        <v>1</v>
+      </c>
+      <c r="M91" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I92" t="b">
+        <v>1</v>
+      </c>
+      <c r="M92" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I93" t="b">
+        <v>1</v>
+      </c>
+      <c r="M93" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I94" t="b">
+        <v>1</v>
+      </c>
+      <c r="M94" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I95" t="b">
+        <v>1</v>
+      </c>
+      <c r="M95" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I96" t="b">
+        <v>1</v>
+      </c>
+      <c r="M96" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I97" t="b">
+        <v>1</v>
+      </c>
+      <c r="M97" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I98" t="b">
+        <v>1</v>
+      </c>
+      <c r="M98" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I99" t="b">
+        <v>1</v>
+      </c>
+      <c r="M99" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I100" t="b">
+        <v>1</v>
+      </c>
+      <c r="M100" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I101" t="b">
+        <v>1</v>
+      </c>
+      <c r="M101" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I102" t="b">
+        <v>1</v>
+      </c>
+      <c r="M102" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I103" t="b">
+        <v>1</v>
+      </c>
+      <c r="M103" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I104" t="b">
+        <v>1</v>
+      </c>
+      <c r="M104" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I105" t="b">
+        <v>1</v>
+      </c>
+      <c r="M105" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I106" t="b">
+        <v>1</v>
+      </c>
+      <c r="M106" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I107" t="b">
+        <v>1</v>
+      </c>
+      <c r="M107" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I108" t="b">
+        <v>1</v>
+      </c>
+      <c r="M108" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I109" t="b">
+        <v>1</v>
+      </c>
+      <c r="M109" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I110" t="b">
+        <v>1</v>
+      </c>
+      <c r="M110" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I111" t="b">
+        <v>1</v>
+      </c>
+      <c r="M111" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I112" t="b">
+        <v>1</v>
+      </c>
+      <c r="M112" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I113" t="b">
+        <v>1</v>
+      </c>
+      <c r="M113" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I114" t="b">
+        <v>1</v>
+      </c>
+      <c r="M114" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I115" t="b">
+        <v>1</v>
+      </c>
+      <c r="M115" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I116" t="b">
+        <v>1</v>
+      </c>
+      <c r="M116" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I117" t="b">
+        <v>1</v>
+      </c>
+      <c r="M117" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I118" t="b">
+        <v>1</v>
+      </c>
+      <c r="M118" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I119" t="b">
+        <v>1</v>
+      </c>
+      <c r="M119" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I120" t="b">
+        <v>1</v>
+      </c>
+      <c r="M120" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I121" t="b">
+        <v>1</v>
+      </c>
+      <c r="M121" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I122" t="b">
+        <v>1</v>
+      </c>
+      <c r="M122" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I123" t="b">
+        <v>1</v>
+      </c>
+      <c r="M123" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I124" t="b">
+        <v>1</v>
+      </c>
+      <c r="M124" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I125" t="b">
+        <v>1</v>
+      </c>
+      <c r="M125" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I126" t="b">
+        <v>1</v>
+      </c>
+      <c r="M126" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I127" t="b">
+        <v>1</v>
+      </c>
+      <c r="M127" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I128" t="b">
+        <v>1</v>
+      </c>
+      <c r="M128" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I129" t="b">
+        <v>1</v>
+      </c>
+      <c r="M129" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I130" t="b">
+        <v>1</v>
+      </c>
+      <c r="M130" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I131" t="b">
+        <v>1</v>
+      </c>
+      <c r="M131" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I132" t="b">
+        <v>1</v>
+      </c>
+      <c r="M132" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I133" t="b">
+        <v>1</v>
+      </c>
+      <c r="M133" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I134" t="b">
+        <v>1</v>
+      </c>
+      <c r="M134" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I135" t="b">
+        <v>1</v>
+      </c>
+      <c r="M135" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I136" t="b">
+        <v>1</v>
+      </c>
+      <c r="M136" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I137" t="b">
+        <v>1</v>
+      </c>
+      <c r="M137" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I138" t="b">
+        <v>1</v>
+      </c>
+      <c r="M138" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I139" t="b">
+        <v>1</v>
+      </c>
+      <c r="M139" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I140" t="b">
+        <v>1</v>
+      </c>
+      <c r="M140" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I141" t="b">
+        <v>1</v>
+      </c>
+      <c r="M141" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I142" t="b">
+        <v>1</v>
+      </c>
+      <c r="M142" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I143" t="b">
+        <v>1</v>
+      </c>
+      <c r="M143" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I144" t="b">
+        <v>1</v>
+      </c>
+      <c r="M144" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I145" t="b">
+        <v>1</v>
+      </c>
+      <c r="M145" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I146" t="b">
+        <v>1</v>
+      </c>
+      <c r="M146" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I147" t="b">
+        <v>1</v>
+      </c>
+      <c r="M147" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I148" t="b">
+        <v>1</v>
+      </c>
+      <c r="M148" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I149" t="b">
+        <v>1</v>
+      </c>
+      <c r="M149" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I150" t="b">
+        <v>1</v>
+      </c>
+      <c r="M150" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I151" t="b">
+        <v>1</v>
+      </c>
+      <c r="M151" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I152" t="b">
+        <v>1</v>
+      </c>
+      <c r="M152" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I153" t="b">
+        <v>1</v>
+      </c>
+      <c r="M153" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I154" t="b">
+        <v>1</v>
+      </c>
+      <c r="M154" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I155" t="b">
+        <v>1</v>
+      </c>
+      <c r="M155" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I156" t="b">
+        <v>1</v>
+      </c>
+      <c r="M156" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I157" t="b">
+        <v>1</v>
+      </c>
+      <c r="M157" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I158" t="b">
+        <v>1</v>
+      </c>
+      <c r="M158" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I159" t="b">
+        <v>1</v>
+      </c>
+      <c r="M159" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I160" t="b">
+        <v>1</v>
+      </c>
+      <c r="M160" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I161" t="b">
+        <v>1</v>
+      </c>
+      <c r="M161" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I162" t="b">
+        <v>1</v>
+      </c>
+      <c r="M162" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I163" t="b">
+        <v>1</v>
+      </c>
+      <c r="M163" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I164" t="b">
+        <v>1</v>
+      </c>
+      <c r="M164" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I165" t="b">
+        <v>1</v>
+      </c>
+      <c r="M165" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I166" t="b">
+        <v>1</v>
+      </c>
+      <c r="M166" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I167" t="b">
+        <v>1</v>
+      </c>
+      <c r="M167" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I168" t="b">
+        <v>1</v>
+      </c>
+      <c r="M168" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I169" t="b">
+        <v>1</v>
+      </c>
+      <c r="M169" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I170" t="b">
+        <v>1</v>
+      </c>
+      <c r="M170" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I171" t="b">
+        <v>1</v>
+      </c>
+      <c r="M171" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I172" t="b">
+        <v>1</v>
+      </c>
+      <c r="M172" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I173" t="b">
+        <v>1</v>
+      </c>
+      <c r="M173" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I174" t="b">
+        <v>1</v>
+      </c>
+      <c r="M174" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I175" t="b">
+        <v>1</v>
+      </c>
+      <c r="M175" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I176" t="b">
+        <v>1</v>
+      </c>
+      <c r="M176" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I177" t="b">
+        <v>1</v>
+      </c>
+      <c r="M177" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I178" t="b">
+        <v>1</v>
+      </c>
+      <c r="M178" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I179" t="b">
+        <v>1</v>
+      </c>
+      <c r="M179" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I180" t="b">
+        <v>1</v>
+      </c>
+      <c r="M180" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I181" t="b">
+        <v>1</v>
+      </c>
+      <c r="M181" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I182" t="b">
+        <v>1</v>
+      </c>
+      <c r="M182" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I183" t="b">
+        <v>1</v>
+      </c>
+      <c r="M183" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I184" t="b">
+        <v>1</v>
+      </c>
+      <c r="M184" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I185" t="b">
+        <v>1</v>
+      </c>
+      <c r="M185" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I186" t="b">
+        <v>1</v>
+      </c>
+      <c r="M186" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I187" t="b">
+        <v>1</v>
+      </c>
+      <c r="M187" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I188" t="b">
+        <v>1</v>
+      </c>
+      <c r="M188" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I189" t="b">
+        <v>1</v>
+      </c>
+      <c r="M189" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I190" t="b">
+        <v>1</v>
+      </c>
+      <c r="M190" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I191" t="b">
+        <v>1</v>
+      </c>
+      <c r="M191" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I192" t="b">
+        <v>1</v>
+      </c>
+      <c r="M192" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I193" t="b">
+        <v>1</v>
+      </c>
+      <c r="M193" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I194" t="b">
+        <v>1</v>
+      </c>
+      <c r="M194" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I195" t="b">
+        <v>1</v>
+      </c>
+      <c r="M195" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I196" t="b">
+        <v>1</v>
+      </c>
+      <c r="M196" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I197" t="b">
+        <v>1</v>
+      </c>
+      <c r="M197" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I198" t="b">
+        <v>1</v>
+      </c>
+      <c r="M198" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I199" t="b">
+        <v>1</v>
+      </c>
+      <c r="M199" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I200" t="b">
+        <v>1</v>
+      </c>
+      <c r="M200" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I201" t="b">
+        <v>1</v>
+      </c>
+      <c r="M201" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I202" t="b">
+        <v>1</v>
+      </c>
+      <c r="M202" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I203" t="b">
+        <v>1</v>
+      </c>
+      <c r="M203" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I204" t="b">
+        <v>1</v>
+      </c>
+      <c r="M204" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I205" t="b">
+        <v>1</v>
+      </c>
+      <c r="M205" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I206" t="b">
+        <v>1</v>
+      </c>
+      <c r="M206" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I207" t="b">
+        <v>1</v>
+      </c>
+      <c r="M207" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I208" t="b">
+        <v>1</v>
+      </c>
+      <c r="M208" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I209" t="b">
+        <v>1</v>
+      </c>
+      <c r="M209" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I210" t="b">
+        <v>1</v>
+      </c>
+      <c r="M210" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I211" t="b">
+        <v>1</v>
+      </c>
+      <c r="M211" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I212" t="b">
+        <v>1</v>
+      </c>
+      <c r="M212" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I213" t="b">
+        <v>1</v>
+      </c>
+      <c r="M213" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I214" t="b">
+        <v>1</v>
+      </c>
+      <c r="M214" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I215" t="b">
+        <v>1</v>
+      </c>
+      <c r="M215" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I216" t="b">
+        <v>1</v>
+      </c>
+      <c r="M216" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I217" t="b">
+        <v>1</v>
+      </c>
+      <c r="M217" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I218" t="b">
+        <v>1</v>
+      </c>
+      <c r="M218" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I219" t="b">
+        <v>1</v>
+      </c>
+      <c r="M219" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I220" t="b">
+        <v>1</v>
+      </c>
+      <c r="M220" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I221" t="b">
+        <v>1</v>
+      </c>
+      <c r="M221" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I222" t="b">
+        <v>1</v>
+      </c>
+      <c r="M222" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I223" t="b">
+        <v>1</v>
+      </c>
+      <c r="M223" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I224" t="b">
+        <v>1</v>
+      </c>
+      <c r="M224" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I225" t="b">
+        <v>1</v>
+      </c>
+      <c r="M225" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I226" t="b">
+        <v>1</v>
+      </c>
+      <c r="M226" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I227" t="b">
+        <v>1</v>
+      </c>
+      <c r="M227" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I228" t="b">
+        <v>1</v>
+      </c>
+      <c r="M228" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I229" t="b">
+        <v>1</v>
+      </c>
+      <c r="M229" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I230" t="b">
+        <v>1</v>
+      </c>
+      <c r="M230" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I231" t="b">
+        <v>1</v>
+      </c>
+      <c r="M231" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I232" t="b">
+        <v>1</v>
+      </c>
+      <c r="M232" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I233" t="b">
+        <v>1</v>
+      </c>
+      <c r="M233" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I234" t="b">
+        <v>1</v>
+      </c>
+      <c r="M234" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I235" t="b">
+        <v>1</v>
+      </c>
+      <c r="M235" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I236" t="b">
+        <v>1</v>
+      </c>
+      <c r="M236" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I237" t="b">
+        <v>1</v>
+      </c>
+      <c r="M237" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I238" t="b">
+        <v>1</v>
+      </c>
+      <c r="M238" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I239" t="b">
+        <v>1</v>
+      </c>
+      <c r="M239" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I240" t="b">
+        <v>1</v>
+      </c>
+      <c r="M240" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I241" t="b">
+        <v>1</v>
+      </c>
+      <c r="M241" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I242" t="b">
+        <v>1</v>
+      </c>
+      <c r="M242" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I243" t="b">
+        <v>1</v>
+      </c>
+      <c r="M243" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I244" t="b">
+        <v>1</v>
+      </c>
+      <c r="M244" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245" spans="9:13" x14ac:dyDescent="0.2">
+      <c r="I245" t="b">
+        <v>1</v>
+      </c>
+      <c r="M245" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="N1:R1"/>
+    <mergeCell ref="U1:W1"/>
+    <mergeCell ref="Y1:Z1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="Y1:Z2">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
+      <formula>"NO"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:D43">
+    <cfRule type="expression" dxfId="7" priority="4">
+      <formula>SUMPRODUCT(--EXACT($D$3:$D$43,$D3))&gt;1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:L43">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N3:S43">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T3:T43">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0618E008-3FD7-DF4B-B9A4-14231511785C}">
+  <dimension ref="B3:E11"/>
+  <sheetViews>
+    <sheetView zoomScale="400" zoomScaleNormal="400" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>441</v>
+      </c>
+      <c r="D4" t="s">
+        <v>230</v>
+      </c>
+      <c r="E4" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>440</v>
+      </c>
+      <c r="C5">
+        <f>COUNTIF(Uncertainty!T3:T43,"TRUE")-COUNTA(Uncertainty!U3:U43)</f>
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <f>COUNTIF(Uncertainty!T3:T43,"TRUE")</f>
+        <v>1</v>
+      </c>
+      <c r="E5" s="14">
+        <f>C5/D5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E6" s="14"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>437</v>
+      </c>
+      <c r="D9" t="s">
+        <v>230</v>
+      </c>
+      <c r="E9" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>202</v>
+      </c>
+      <c r="C10">
+        <f>COUNTIF(Uncertainty!Y:Y,"NO")</f>
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <f>COUNTA(Uncertainty!Y:Y)-2</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="14" t="e">
+        <f>C10/D10</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>436</v>
+      </c>
+      <c r="C11">
+        <f>COUNTIF(Uncertainty!Z:Z,"NO")</f>
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <f>COUNTA(Uncertainty!Y:Y)-2</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="14" t="e">
+        <f>C11/D11</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D5 D10:D11">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>NOT(AND($D$5=$D$10,$D$5=$D$11))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
sota RQ2 - structure
</commit_message>
<xml_diff>
--- a/sota/src/data.xlsx
+++ b/sota/src/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ludovic/Documents/thesis/sota/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1984CA5B-1ED2-714B-9376-5804923BB0BE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD9EF826-B5A4-284F-982C-CCAA88DDEAB7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="-10340" windowWidth="51200" windowHeight="28340" activeTab="2" xr2:uid="{A557A50A-5DDC-A947-B4B9-80A2CEF9B354}"/>
   </bookViews>
@@ -3123,9 +3123,6 @@
     <t>M. Carbin, S. Misailovic, and M. C. Rinard</t>
   </si>
   <si>
-    <t>Verifying quantitative reliability of programs that execute on unreliable hardware</t>
-  </si>
-  <si>
     <t>https://doi.org/10.1145/2509136.2509546</t>
   </si>
   <si>
@@ -4156,6 +4153,9 @@
   </si>
   <si>
     <t>Rainbow:  Architecture-based  self-adaptation  with  reusable  infrastructure</t>
+  </si>
+  <si>
+    <t>Verifying quantitative reliability for programs that execute on unreliable hardware</t>
   </si>
 </sst>
 </file>
@@ -4214,7 +4214,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4278,6 +4278,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4890,27 +4893,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
-      <c r="J1" s="24" t="s">
+      <c r="J1" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="N1" s="24" t="s">
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="N1" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="24"/>
-      <c r="U1" s="24" t="s">
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="U1" s="25" t="s">
         <v>198</v>
       </c>
-      <c r="V1" s="24"/>
-      <c r="W1" s="24"/>
-      <c r="Y1" s="24" t="s">
+      <c r="V1" s="25"/>
+      <c r="W1" s="25"/>
+      <c r="Y1" s="25" t="s">
         <v>205</v>
       </c>
-      <c r="Z1" s="24"/>
+      <c r="Z1" s="25"/>
     </row>
     <row r="2" spans="1:26">
       <c r="A2" s="2" t="s">
@@ -13124,7 +13127,7 @@
         <v>416</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
       <c r="D123" s="8" t="str">
         <f t="shared" si="5"/>
@@ -13282,7 +13285,7 @@
         <v>419</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
       <c r="D125" s="8" t="str">
         <f t="shared" si="5"/>
@@ -14360,7 +14363,7 @@
         <v>536</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="D141" s="15" t="str">
         <f t="shared" si="5"/>
@@ -25096,10 +25099,10 @@
   <dimension ref="A1:Z245"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="S37" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="R101" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="V69" sqref="V69"/>
+      <selection pane="bottomRight" activeCell="U125" sqref="U125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -25119,27 +25122,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
-      <c r="J1" s="25" t="s">
+      <c r="J1" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="N1" s="25" t="s">
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="N1" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="U1" s="25" t="s">
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="U1" s="26" t="s">
         <v>198</v>
       </c>
-      <c r="V1" s="25"/>
-      <c r="W1" s="25"/>
-      <c r="Y1" s="25" t="s">
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="Y1" s="26" t="s">
         <v>205</v>
       </c>
-      <c r="Z1" s="25"/>
+      <c r="Z1" s="26"/>
     </row>
     <row r="2" spans="1:26">
       <c r="A2" s="9" t="s">
@@ -25203,13 +25206,13 @@
         <v>11</v>
       </c>
       <c r="U2" s="9" t="s">
+        <v>1360</v>
+      </c>
+      <c r="V2" s="9" t="s">
         <v>1361</v>
       </c>
-      <c r="V2" s="9" t="s">
+      <c r="W2" s="9" t="s">
         <v>1362</v>
-      </c>
-      <c r="W2" s="9" t="s">
-        <v>1363</v>
       </c>
       <c r="X2" s="9" t="s">
         <v>12</v>
@@ -27798,7 +27801,7 @@
         <v>887</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
       <c r="D40" s="9" t="str">
         <f t="shared" si="0"/>
@@ -29172,7 +29175,7 @@
         <v>961</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="D61" s="9" t="str">
         <f t="shared" si="0"/>
@@ -30020,7 +30023,7 @@
         <v>999</v>
       </c>
       <c r="C75" s="18" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="D75" s="9" t="str">
         <f t="shared" si="3"/>
@@ -30580,12 +30583,12 @@
       <c r="B84" s="9" t="s">
         <v>1028</v>
       </c>
-      <c r="C84" s="9" t="s">
-        <v>1029</v>
+      <c r="C84" s="24" t="s">
+        <v>1366</v>
       </c>
       <c r="D84" s="18" t="str">
         <f t="shared" si="3"/>
-        <v>verifying quantitative reliability of programs that execute on unreliable hardware</v>
+        <v>verifying quantitative reliability for programs that execute on unreliable hardware</v>
       </c>
       <c r="E84" s="9" t="s">
         <v>841</v>
@@ -30594,7 +30597,7 @@
         <v>2013</v>
       </c>
       <c r="G84" s="13" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="H84" s="18" t="s">
         <v>229</v>
@@ -30657,23 +30660,23 @@
         <v>83</v>
       </c>
       <c r="B85" s="9" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C85" s="9" t="s">
         <v>1031</v>
-      </c>
-      <c r="C85" s="9" t="s">
-        <v>1032</v>
       </c>
       <c r="D85" s="18" t="str">
         <f t="shared" si="3"/>
         <v>efficiently sampling probabilistic programs via program analysis</v>
       </c>
       <c r="E85" s="9" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="F85" s="9">
         <v>2013</v>
       </c>
       <c r="G85" s="13" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="H85" s="18" t="s">
         <v>229</v>
@@ -30736,23 +30739,23 @@
         <v>84</v>
       </c>
       <c r="B86" s="9" t="s">
+        <v>1034</v>
+      </c>
+      <c r="C86" s="9" t="s">
         <v>1035</v>
-      </c>
-      <c r="C86" s="9" t="s">
-        <v>1036</v>
       </c>
       <c r="D86" s="18" t="str">
         <f t="shared" si="3"/>
         <v>management of probabilistic data: foundations and challenges</v>
       </c>
       <c r="E86" s="9" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="F86" s="9">
         <v>2007</v>
       </c>
       <c r="G86" s="13" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="H86" s="18" t="s">
         <v>229</v>
@@ -30800,23 +30803,23 @@
         <v>85</v>
       </c>
       <c r="B87" s="9" t="s">
+        <v>1038</v>
+      </c>
+      <c r="C87" s="9" t="s">
         <v>1039</v>
-      </c>
-      <c r="C87" s="9" t="s">
-        <v>1040</v>
       </c>
       <c r="D87" s="18" t="str">
         <f t="shared" si="3"/>
         <v>neural acceleration for general-purpose approximate programs</v>
       </c>
       <c r="E87" s="9" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="F87" s="9">
         <v>2012</v>
       </c>
       <c r="G87" s="13" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="H87" s="18" t="s">
         <v>229</v>
@@ -30864,10 +30867,10 @@
         <v>86</v>
       </c>
       <c r="B88" s="9" t="s">
+        <v>1042</v>
+      </c>
+      <c r="C88" s="9" t="s">
         <v>1043</v>
-      </c>
-      <c r="C88" s="9" t="s">
-        <v>1044</v>
       </c>
       <c r="D88" s="18" t="str">
         <f t="shared" si="3"/>
@@ -30880,7 +30883,7 @@
         <v>1994</v>
       </c>
       <c r="G88" s="13" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="H88" s="18" t="s">
         <v>229</v>
@@ -30928,23 +30931,23 @@
         <v>87</v>
       </c>
       <c r="B89" s="9" t="s">
+        <v>1045</v>
+      </c>
+      <c r="C89" s="9" t="s">
         <v>1046</v>
-      </c>
-      <c r="C89" s="9" t="s">
-        <v>1047</v>
       </c>
       <c r="D89" s="18" t="str">
         <f t="shared" si="3"/>
         <v>a categorical approach to probability theory</v>
       </c>
       <c r="E89" s="9" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="F89" s="9">
         <v>1982</v>
       </c>
       <c r="G89" s="13" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="H89" s="18" t="s">
         <v>229</v>
@@ -30992,23 +30995,23 @@
         <v>88</v>
       </c>
       <c r="B90" s="9" t="s">
+        <v>1049</v>
+      </c>
+      <c r="C90" s="9" t="s">
         <v>1050</v>
-      </c>
-      <c r="C90" s="9" t="s">
-        <v>1051</v>
       </c>
       <c r="D90" s="18" t="str">
         <f t="shared" si="3"/>
         <v>church: a language for generative models</v>
       </c>
       <c r="E90" s="9" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="F90" s="9">
         <v>2008</v>
       </c>
       <c r="G90" s="13" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="H90" s="18" t="s">
         <v>229</v>
@@ -31056,23 +31059,23 @@
         <v>89</v>
       </c>
       <c r="B91" s="9" t="s">
+        <v>1053</v>
+      </c>
+      <c r="C91" s="9" t="s">
         <v>1054</v>
-      </c>
-      <c r="C91" s="9" t="s">
-        <v>1055</v>
       </c>
       <c r="D91" s="18" t="str">
         <f t="shared" si="3"/>
         <v>arithmetic operations on independent random variables: a numerical approach</v>
       </c>
       <c r="E91" s="9" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="F91" s="9">
         <v>2012</v>
       </c>
       <c r="G91" s="13" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="H91" s="18" t="s">
         <v>229</v>
@@ -31115,10 +31118,10 @@
         <v>1</v>
       </c>
       <c r="U91" s="9" t="s">
-        <v>229</v>
+        <v>17</v>
       </c>
       <c r="V91" s="9" t="s">
-        <v>229</v>
+        <v>17</v>
       </c>
       <c r="W91" s="9" t="s">
         <v>225</v>
@@ -31135,23 +31138,23 @@
         <v>90</v>
       </c>
       <c r="B92" s="9" t="s">
+        <v>1057</v>
+      </c>
+      <c r="C92" s="9" t="s">
         <v>1058</v>
-      </c>
-      <c r="C92" s="9" t="s">
-        <v>1059</v>
       </c>
       <c r="D92" s="18" t="str">
         <f t="shared" si="3"/>
         <v>group sequential methods with applications to clinical trials</v>
       </c>
       <c r="E92" s="9" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="F92" s="9">
         <v>2000</v>
       </c>
       <c r="G92" s="13" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="H92" s="18" t="s">
         <v>229</v>
@@ -31199,10 +31202,10 @@
         <v>91</v>
       </c>
       <c r="B93" s="9" t="s">
+        <v>1061</v>
+      </c>
+      <c r="C93" s="9" t="s">
         <v>1062</v>
-      </c>
-      <c r="C93" s="9" t="s">
-        <v>1063</v>
       </c>
       <c r="D93" s="18" t="str">
         <f t="shared" si="3"/>
@@ -31215,7 +31218,7 @@
         <v>2013</v>
       </c>
       <c r="G93" s="13" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="H93" s="18" t="s">
         <v>229</v>
@@ -31263,23 +31266,23 @@
         <v>92</v>
       </c>
       <c r="B94" s="9" t="s">
+        <v>1064</v>
+      </c>
+      <c r="C94" s="9" t="s">
         <v>1065</v>
-      </c>
-      <c r="C94" s="9" t="s">
-        <v>1066</v>
       </c>
       <c r="D94" s="18" t="str">
         <f t="shared" si="3"/>
         <v>interval analysis</v>
       </c>
       <c r="E94" s="9" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="F94" s="9">
         <v>1966</v>
       </c>
       <c r="G94" s="13" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="H94" s="18" t="s">
         <v>229</v>
@@ -31327,23 +31330,23 @@
         <v>93</v>
       </c>
       <c r="B95" s="9" t="s">
+        <v>1068</v>
+      </c>
+      <c r="C95" s="9" t="s">
         <v>1069</v>
-      </c>
-      <c r="C95" s="9" t="s">
-        <v>1070</v>
       </c>
       <c r="D95" s="18" t="str">
         <f t="shared" si="3"/>
         <v>bayesian learning for neural networks</v>
       </c>
       <c r="E95" s="9" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="F95" s="9">
         <v>1994</v>
       </c>
       <c r="G95" s="13" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="H95" s="18" t="s">
         <v>229</v>
@@ -31391,23 +31394,23 @@
         <v>94</v>
       </c>
       <c r="B96" s="9" t="s">
+        <v>1072</v>
+      </c>
+      <c r="C96" s="9" t="s">
         <v>1073</v>
-      </c>
-      <c r="C96" s="9" t="s">
-        <v>1074</v>
       </c>
       <c r="D96" s="18" t="str">
         <f t="shared" si="3"/>
         <v>hidden markov map matching through noise and sparseness</v>
       </c>
       <c r="E96" s="9" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="F96" s="9">
         <v>2009</v>
       </c>
       <c r="G96" s="13" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="H96" s="18" t="s">
         <v>229</v>
@@ -31455,10 +31458,10 @@
         <v>95</v>
       </c>
       <c r="B97" s="9" t="s">
+        <v>1076</v>
+      </c>
+      <c r="C97" s="9" t="s">
         <v>1077</v>
-      </c>
-      <c r="C97" s="9" t="s">
-        <v>1078</v>
       </c>
       <c r="D97" s="18" t="str">
         <f t="shared" si="3"/>
@@ -31513,10 +31516,10 @@
         <v>96</v>
       </c>
       <c r="B98" s="9" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C98" s="9" t="s">
         <v>1079</v>
-      </c>
-      <c r="C98" s="9" t="s">
-        <v>1080</v>
       </c>
       <c r="D98" s="18" t="str">
         <f t="shared" si="3"/>
@@ -31529,7 +31532,7 @@
         <v>2005</v>
       </c>
       <c r="G98" s="13" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="H98" s="18" t="s">
         <v>229</v>
@@ -31592,10 +31595,10 @@
         <v>97</v>
       </c>
       <c r="B99" s="9" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C99" s="9" t="s">
         <v>1082</v>
-      </c>
-      <c r="C99" s="9" t="s">
-        <v>1083</v>
       </c>
       <c r="D99" s="18" t="str">
         <f t="shared" si="3"/>
@@ -31608,7 +31611,7 @@
         <v>2001</v>
       </c>
       <c r="G99" s="13" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="H99" s="18" t="s">
         <v>229</v>
@@ -31671,10 +31674,10 @@
         <v>98</v>
       </c>
       <c r="B100" s="9" t="s">
+        <v>1084</v>
+      </c>
+      <c r="C100" s="9" t="s">
         <v>1085</v>
-      </c>
-      <c r="C100" s="9" t="s">
-        <v>1086</v>
       </c>
       <c r="D100" s="18" t="str">
         <f t="shared" si="3"/>
@@ -31687,7 +31690,7 @@
         <v>2002</v>
       </c>
       <c r="G100" s="13" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="H100" s="18" t="s">
         <v>229</v>
@@ -31750,23 +31753,23 @@
         <v>99</v>
       </c>
       <c r="B101" s="9" t="s">
+        <v>1087</v>
+      </c>
+      <c r="C101" s="9" t="s">
         <v>1088</v>
-      </c>
-      <c r="C101" s="9" t="s">
-        <v>1089</v>
       </c>
       <c r="D101" s="18" t="str">
         <f t="shared" si="3"/>
         <v>enerj: approximate data types for safe and general low-power computation</v>
       </c>
       <c r="E101" s="9" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="F101" s="9">
         <v>2011</v>
       </c>
       <c r="G101" s="13" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="H101" s="18" t="s">
         <v>229</v>
@@ -31814,23 +31817,23 @@
         <v>100</v>
       </c>
       <c r="B102" s="9" t="s">
+        <v>1091</v>
+      </c>
+      <c r="C102" s="9" t="s">
         <v>1092</v>
-      </c>
-      <c r="C102" s="9" t="s">
-        <v>1093</v>
       </c>
       <c r="D102" s="18" t="str">
         <f t="shared" si="3"/>
         <v>static analysis for probabilistic programs: inferring whole program properties from finitely many paths</v>
       </c>
       <c r="E102" s="9" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="F102" s="9">
         <v>2013</v>
       </c>
       <c r="G102" s="13" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="H102" s="18" t="s">
         <v>229</v>
@@ -31893,23 +31896,23 @@
         <v>101</v>
       </c>
       <c r="B103" s="9" t="s">
+        <v>1094</v>
+      </c>
+      <c r="C103" s="9" t="s">
         <v>1095</v>
-      </c>
-      <c r="C103" s="9" t="s">
-        <v>1096</v>
       </c>
       <c r="D103" s="18" t="str">
         <f t="shared" si="3"/>
         <v>monte carlo methods for managing interactive state, action and feedback under uncertainty</v>
       </c>
       <c r="E103" s="9" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="F103" s="9">
         <v>2011</v>
       </c>
       <c r="G103" s="13" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="H103" s="18" t="s">
         <v>229</v>
@@ -31972,23 +31975,23 @@
         <v>102</v>
       </c>
       <c r="B104" s="9" t="s">
+        <v>1098</v>
+      </c>
+      <c r="C104" s="9" t="s">
         <v>1099</v>
-      </c>
-      <c r="C104" s="9" t="s">
-        <v>1100</v>
       </c>
       <c r="D104" s="18" t="str">
         <f t="shared" si="3"/>
         <v>global positioning system: the mathematics of gps receivers</v>
       </c>
       <c r="E104" s="9" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="F104" s="9">
         <v>1998</v>
       </c>
       <c r="G104" s="13" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="H104" s="18" t="s">
         <v>229</v>
@@ -32036,23 +32039,23 @@
         <v>103</v>
       </c>
       <c r="B105" s="9" t="s">
+        <v>1102</v>
+      </c>
+      <c r="C105" s="9" t="s">
         <v>1103</v>
-      </c>
-      <c r="C105" s="9" t="s">
-        <v>1104</v>
       </c>
       <c r="D105" s="18" t="str">
         <f t="shared" si="3"/>
         <v>towards programming tools for robots that integrate probabilistic computation and learning</v>
       </c>
       <c r="E105" s="9" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="F105" s="9">
         <v>2000</v>
       </c>
       <c r="G105" s="13" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="H105" s="18" t="s">
         <v>229</v>
@@ -32115,10 +32118,10 @@
         <v>104</v>
       </c>
       <c r="B106" s="9" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C106" s="9" t="s">
         <v>1107</v>
-      </c>
-      <c r="C106" s="9" t="s">
-        <v>1108</v>
       </c>
       <c r="D106" s="18" t="str">
         <f t="shared" si="3"/>
@@ -32128,7 +32131,7 @@
         <v>1970</v>
       </c>
       <c r="G106" s="13" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="H106" s="18" t="s">
         <v>229</v>
@@ -32176,17 +32179,17 @@
         <v>105</v>
       </c>
       <c r="B107" s="9" t="s">
+        <v>1109</v>
+      </c>
+      <c r="C107" s="9" t="s">
         <v>1110</v>
-      </c>
-      <c r="C107" s="9" t="s">
-        <v>1111</v>
       </c>
       <c r="D107" s="18" t="str">
         <f t="shared" si="3"/>
         <v>sequential tests of statistical hypotheses</v>
       </c>
       <c r="E107" s="9" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="F107" s="9">
         <v>1945</v>
@@ -32237,10 +32240,10 @@
         <v>106</v>
       </c>
       <c r="B108" s="9" t="s">
+        <v>1112</v>
+      </c>
+      <c r="C108" s="9" t="s">
         <v>1113</v>
-      </c>
-      <c r="C108" s="9" t="s">
-        <v>1114</v>
       </c>
       <c r="D108" s="18" t="str">
         <f t="shared" si="3"/>
@@ -32250,7 +32253,7 @@
         <v>2016</v>
       </c>
       <c r="G108" s="13" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="H108" s="9" t="s">
         <v>229</v>
@@ -32298,10 +32301,10 @@
         <v>107</v>
       </c>
       <c r="B109" s="9" t="s">
+        <v>1115</v>
+      </c>
+      <c r="C109" s="9" t="s">
         <v>1116</v>
-      </c>
-      <c r="C109" s="9" t="s">
-        <v>1117</v>
       </c>
       <c r="D109" s="9" t="str">
         <f t="shared" si="3"/>
@@ -32311,7 +32314,7 @@
         <v>2015</v>
       </c>
       <c r="G109" s="13" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="H109" s="19" t="s">
         <v>229</v>
@@ -32359,10 +32362,10 @@
         <v>108</v>
       </c>
       <c r="B110" s="9" t="s">
+        <v>1118</v>
+      </c>
+      <c r="C110" s="9" t="s">
         <v>1119</v>
-      </c>
-      <c r="C110" s="9" t="s">
-        <v>1120</v>
       </c>
       <c r="D110" s="9" t="str">
         <f t="shared" si="3"/>
@@ -32372,7 +32375,7 @@
         <v>2009</v>
       </c>
       <c r="G110" s="13" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="H110" s="19" t="s">
         <v>229</v>
@@ -32420,23 +32423,23 @@
         <v>109</v>
       </c>
       <c r="B111" s="9" t="s">
+        <v>1121</v>
+      </c>
+      <c r="C111" s="9" t="s">
         <v>1122</v>
-      </c>
-      <c r="C111" s="9" t="s">
-        <v>1123</v>
       </c>
       <c r="D111" s="9" t="str">
         <f t="shared" si="3"/>
         <v>cvode, a stiff/nonstiff ode solver in c</v>
       </c>
       <c r="E111" s="9" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="F111" s="9">
         <v>1996</v>
       </c>
       <c r="G111" s="13" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="H111" s="19" t="s">
         <v>229</v>
@@ -32484,10 +32487,10 @@
         <v>110</v>
       </c>
       <c r="B112" s="9" t="s">
+        <v>1125</v>
+      </c>
+      <c r="C112" s="9" t="s">
         <v>1126</v>
-      </c>
-      <c r="C112" s="9" t="s">
-        <v>1127</v>
       </c>
       <c r="D112" s="9" t="str">
         <f t="shared" si="3"/>
@@ -32497,7 +32500,7 @@
         <v>2010</v>
       </c>
       <c r="G112" s="13" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="H112" s="19" t="s">
         <v>229</v>
@@ -32545,23 +32548,23 @@
         <v>111</v>
       </c>
       <c r="B113" s="9" t="s">
+        <v>1128</v>
+      </c>
+      <c r="C113" s="9" t="s">
         <v>1129</v>
-      </c>
-      <c r="C113" s="9" t="s">
-        <v>1130</v>
       </c>
       <c r="D113" s="9" t="str">
         <f t="shared" si="3"/>
         <v>hybrid monte carlo</v>
       </c>
       <c r="E113" s="9" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="F113" s="9">
         <v>1987</v>
       </c>
       <c r="G113" s="13" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="H113" s="19" t="s">
         <v>229</v>
@@ -32609,10 +32612,10 @@
         <v>112</v>
       </c>
       <c r="B114" s="9" t="s">
+        <v>1132</v>
+      </c>
+      <c r="C114" s="9" t="s">
         <v>1133</v>
-      </c>
-      <c r="C114" s="9" t="s">
-        <v>1134</v>
       </c>
       <c r="D114" s="9" t="str">
         <f t="shared" si="3"/>
@@ -32667,23 +32670,23 @@
         <v>113</v>
       </c>
       <c r="B115" s="9" t="s">
+        <v>1134</v>
+      </c>
+      <c r="C115" s="9" t="s">
         <v>1135</v>
-      </c>
-      <c r="C115" s="9" t="s">
-        <v>1136</v>
       </c>
       <c r="D115" s="9" t="str">
         <f t="shared" si="3"/>
         <v>bayesian data analysis</v>
       </c>
       <c r="E115" s="9" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="F115" s="9">
         <v>2013</v>
       </c>
       <c r="G115" s="13" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="H115" s="19" t="s">
         <v>229</v>
@@ -32731,23 +32734,23 @@
         <v>114</v>
       </c>
       <c r="B116" s="9" t="s">
+        <v>1138</v>
+      </c>
+      <c r="C116" s="9" t="s">
         <v>1139</v>
-      </c>
-      <c r="C116" s="9" t="s">
-        <v>1140</v>
       </c>
       <c r="D116" s="9" t="str">
         <f t="shared" si="3"/>
         <v>why we (usually) don’t have to worry about multiple comparisons</v>
       </c>
       <c r="E116" s="9" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="F116" s="9">
         <v>2012</v>
       </c>
       <c r="G116" s="13" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="H116" s="19" t="s">
         <v>229</v>
@@ -32795,23 +32798,23 @@
         <v>115</v>
       </c>
       <c r="B117" s="9" t="s">
+        <v>1142</v>
+      </c>
+      <c r="C117" s="9" t="s">
         <v>1143</v>
-      </c>
-      <c r="C117" s="9" t="s">
-        <v>1144</v>
       </c>
       <c r="D117" s="9" t="str">
         <f t="shared" si="3"/>
         <v>inference from iterative simulation using multiple sequences</v>
       </c>
       <c r="E117" s="9" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="F117" s="9">
         <v>1992</v>
       </c>
       <c r="G117" s="13" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="H117" s="19" t="s">
         <v>229</v>
@@ -32859,23 +32862,23 @@
         <v>116</v>
       </c>
       <c r="B118" s="9" t="s">
+        <v>1146</v>
+      </c>
+      <c r="C118" s="9" t="s">
         <v>1147</v>
-      </c>
-      <c r="C118" s="9" t="s">
-        <v>1148</v>
       </c>
       <c r="D118" s="9" t="str">
         <f t="shared" si="3"/>
         <v>introduction to markov chain monte carlo</v>
       </c>
       <c r="E118" s="9" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="F118" s="9">
         <v>2011</v>
       </c>
       <c r="G118" s="13" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="H118" s="19" t="s">
         <v>229</v>
@@ -32923,10 +32926,10 @@
         <v>117</v>
       </c>
       <c r="B119" s="9" t="s">
+        <v>1150</v>
+      </c>
+      <c r="C119" s="9" t="s">
         <v>1151</v>
-      </c>
-      <c r="C119" s="9" t="s">
-        <v>1152</v>
       </c>
       <c r="D119" s="9" t="str">
         <f t="shared" si="3"/>
@@ -32936,7 +32939,7 @@
         <v>2016</v>
       </c>
       <c r="G119" s="13" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="H119" s="19" t="s">
         <v>229</v>
@@ -32984,10 +32987,10 @@
         <v>118</v>
       </c>
       <c r="B120" s="9" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="C120" s="9" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="D120" s="9" t="str">
         <f t="shared" si="3"/>
@@ -32997,7 +33000,7 @@
         <v>2010</v>
       </c>
       <c r="G120" s="13" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="H120" s="19" t="s">
         <v>229</v>
@@ -33045,23 +33048,23 @@
         <v>119</v>
       </c>
       <c r="B121" s="9" t="s">
+        <v>1156</v>
+      </c>
+      <c r="C121" s="9" t="s">
         <v>1157</v>
-      </c>
-      <c r="C121" s="9" t="s">
-        <v>1158</v>
       </c>
       <c r="D121" s="9" t="str">
         <f t="shared" si="3"/>
         <v>sundials: suite of nonlinear and differential/algebraic equation solvers</v>
       </c>
       <c r="E121" s="9" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="F121" s="9">
         <v>2005</v>
       </c>
       <c r="G121" s="13" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="H121" s="19" t="s">
         <v>229</v>
@@ -33109,23 +33112,23 @@
         <v>120</v>
       </c>
       <c r="B122" s="9" t="s">
+        <v>1160</v>
+      </c>
+      <c r="C122" s="9" t="s">
         <v>1161</v>
-      </c>
-      <c r="C122" s="9" t="s">
-        <v>1162</v>
       </c>
       <c r="D122" s="9" t="str">
         <f t="shared" si="3"/>
         <v>the no-u-turn sampler: adaptively setting path lengths in hamiltonian monte carlo</v>
       </c>
       <c r="E122" s="9" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="F122" s="9">
         <v>2014</v>
       </c>
       <c r="G122" s="13" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="H122" s="19" t="s">
         <v>229</v>
@@ -33173,23 +33176,23 @@
         <v>121</v>
       </c>
       <c r="B123" s="9" t="s">
+        <v>1164</v>
+      </c>
+      <c r="C123" s="9" t="s">
         <v>1165</v>
-      </c>
-      <c r="C123" s="9" t="s">
-        <v>1166</v>
       </c>
       <c r="D123" s="9" t="str">
         <f t="shared" si="3"/>
         <v>the bugs book – a practical introduction to bayesian analysis</v>
       </c>
       <c r="E123" s="9" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="F123" s="9">
         <v>2012</v>
       </c>
       <c r="G123" s="13" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="H123" s="19" t="s">
         <v>229</v>
@@ -33237,23 +33240,23 @@
         <v>122</v>
       </c>
       <c r="B124" s="9" t="s">
+        <v>1167</v>
+      </c>
+      <c r="C124" s="9" t="s">
         <v>1168</v>
-      </c>
-      <c r="C124" s="9" t="s">
-        <v>1169</v>
       </c>
       <c r="D124" s="9" t="str">
         <f t="shared" si="3"/>
         <v>the bugs project: evolution, critique, and future directions</v>
       </c>
       <c r="E124" s="9" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="F124" s="9">
         <v>2009</v>
       </c>
       <c r="G124" s="13" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="H124" s="19" t="s">
         <v>229</v>
@@ -33301,23 +33304,23 @@
         <v>123</v>
       </c>
       <c r="B125" s="9" t="s">
+        <v>1171</v>
+      </c>
+      <c r="C125" s="9" t="s">
         <v>1172</v>
-      </c>
-      <c r="C125" s="9" t="s">
-        <v>1173</v>
       </c>
       <c r="D125" s="9" t="str">
         <f t="shared" si="3"/>
         <v>winbugs – a bayesian modelling framework: concepts, structure, and extensibility</v>
       </c>
       <c r="E125" s="9" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="F125" s="9">
         <v>2000</v>
       </c>
       <c r="G125" s="13" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="H125" s="19" t="s">
         <v>229</v>
@@ -33360,7 +33363,7 @@
         <v>1</v>
       </c>
       <c r="U125" s="21" t="s">
-        <v>229</v>
+        <v>17</v>
       </c>
       <c r="V125" s="21" t="s">
         <v>225</v>
@@ -33380,23 +33383,23 @@
         <v>124</v>
       </c>
       <c r="B126" s="9" t="s">
+        <v>1175</v>
+      </c>
+      <c r="C126" s="9" t="s">
         <v>1176</v>
-      </c>
-      <c r="C126" s="9" t="s">
-        <v>1177</v>
       </c>
       <c r="D126" s="9" t="str">
         <f t="shared" si="3"/>
         <v>equation of state calculations by fast computing machines</v>
       </c>
       <c r="E126" s="9" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="F126" s="9">
         <v>1953</v>
       </c>
       <c r="G126" s="13" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="H126" s="19" t="s">
         <v>229</v>
@@ -33444,17 +33447,17 @@
         <v>125</v>
       </c>
       <c r="B127" s="9" t="s">
+        <v>1179</v>
+      </c>
+      <c r="C127" s="9" t="s">
         <v>1180</v>
-      </c>
-      <c r="C127" s="9" t="s">
-        <v>1181</v>
       </c>
       <c r="D127" s="9" t="str">
         <f t="shared" si="3"/>
         <v>the latex companion. tools and techniques for computer typesetting</v>
       </c>
       <c r="E127" s="9" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="F127" s="9">
         <v>2004</v>
@@ -33506,23 +33509,23 @@
         <v>126</v>
       </c>
       <c r="B128" s="9" t="s">
+        <v>1182</v>
+      </c>
+      <c r="C128" s="9" t="s">
         <v>1183</v>
-      </c>
-      <c r="C128" s="9" t="s">
-        <v>1184</v>
       </c>
       <c r="D128" s="9" t="str">
         <f t="shared" si="3"/>
         <v>mcmc using hamiltonian dynamics.</v>
       </c>
       <c r="E128" s="9" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="F128" s="9">
         <v>2011</v>
       </c>
       <c r="G128" s="13" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="H128" s="19" t="s">
         <v>229</v>
@@ -33570,23 +33573,23 @@
         <v>127</v>
       </c>
       <c r="B129" s="9" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C129" s="9" t="s">
         <v>1186</v>
-      </c>
-      <c r="C129" s="9" t="s">
-        <v>1187</v>
       </c>
       <c r="D129" s="9" t="str">
         <f t="shared" si="3"/>
         <v>an improved acceptance procedure for the hybrid monte carlo algo- rithm</v>
       </c>
       <c r="E129" s="9" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="F129" s="9">
         <v>1994</v>
       </c>
       <c r="G129" s="13" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="H129" s="19" t="s">
         <v>229</v>
@@ -33634,23 +33637,23 @@
         <v>128</v>
       </c>
       <c r="B130" s="9" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="C130" s="9" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="D130" s="9" t="str">
         <f t="shared" si="3"/>
         <v>slice sampling</v>
       </c>
       <c r="E130" s="9" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="F130" s="9">
         <v>2003</v>
       </c>
       <c r="G130" s="13" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="H130" s="19" t="s">
         <v>229</v>
@@ -33698,17 +33701,17 @@
         <v>129</v>
       </c>
       <c r="B131" s="9" t="s">
+        <v>1191</v>
+      </c>
+      <c r="C131" s="9" t="s">
         <v>1192</v>
-      </c>
-      <c r="C131" s="9" t="s">
-        <v>1193</v>
       </c>
       <c r="D131" s="9" t="str">
         <f t="shared" si="3"/>
         <v>numerical optimization</v>
       </c>
       <c r="E131" s="9" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="F131" s="9">
         <v>2006</v>
@@ -33759,23 +33762,23 @@
         <v>130</v>
       </c>
       <c r="B132" s="9" t="s">
+        <v>1194</v>
+      </c>
+      <c r="C132" s="9" t="s">
         <v>1195</v>
-      </c>
-      <c r="C132" s="9" t="s">
-        <v>1196</v>
       </c>
       <c r="D132" s="9" t="str">
         <f t="shared" si="3"/>
         <v>jags: a program for analysis of bayesian graphical models using gibbs sampling</v>
       </c>
       <c r="E132" s="9" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="F132" s="9">
         <v>2003</v>
       </c>
       <c r="G132" s="13" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="H132" s="19" t="s">
         <v>229</v>
@@ -33818,7 +33821,7 @@
         <v>1</v>
       </c>
       <c r="U132" s="9" t="s">
-        <v>229</v>
+        <v>17</v>
       </c>
       <c r="V132" s="9" t="s">
         <v>225</v>
@@ -33838,23 +33841,23 @@
         <v>131</v>
       </c>
       <c r="B133" s="9" t="s">
+        <v>1198</v>
+      </c>
+      <c r="C133" s="9" t="s">
         <v>1199</v>
-      </c>
-      <c r="C133" s="9" t="s">
-        <v>1200</v>
       </c>
       <c r="D133" s="9" t="str">
         <f t="shared" si="3"/>
         <v>code: convergence diagnosis and out- put analysis for mcmc</v>
       </c>
       <c r="E133" s="9" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="F133" s="9">
         <v>2006</v>
       </c>
       <c r="G133" s="13" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="H133" s="19" t="s">
         <v>229</v>
@@ -33902,23 +33905,23 @@
         <v>132</v>
       </c>
       <c r="B134" s="9" t="s">
+        <v>1202</v>
+      </c>
+      <c r="C134" s="9" t="s">
         <v>1203</v>
-      </c>
-      <c r="C134" s="9" t="s">
-        <v>1204</v>
       </c>
       <c r="D134" s="9" t="str">
         <f t="shared" si="3"/>
         <v>r: a language and environment for statistical computing</v>
       </c>
       <c r="E134" s="9" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="F134" s="9">
         <v>2016</v>
       </c>
       <c r="G134" s="13" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="H134" s="19" t="s">
         <v>229</v>
@@ -33966,23 +33969,23 @@
         <v>133</v>
       </c>
       <c r="B135" s="9" t="s">
+        <v>1206</v>
+      </c>
+      <c r="C135" s="9" t="s">
         <v>1207</v>
-      </c>
-      <c r="C135" s="9" t="s">
-        <v>1208</v>
       </c>
       <c r="D135" s="9" t="str">
         <f t="shared" si="3"/>
         <v>the boost c++ libraries</v>
       </c>
       <c r="E135" s="9" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="F135" s="9">
         <v>2011</v>
       </c>
       <c r="G135" s="13" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="H135" s="19" t="s">
         <v>229</v>
@@ -34030,23 +34033,23 @@
         <v>134</v>
       </c>
       <c r="B136" s="9" t="s">
+        <v>1210</v>
+      </c>
+      <c r="C136" s="9" t="s">
         <v>1211</v>
-      </c>
-      <c r="C136" s="9" t="s">
-        <v>1212</v>
       </c>
       <c r="D136" s="9" t="str">
         <f t="shared" si="3"/>
         <v>jenkins: the definitive guide</v>
       </c>
       <c r="E136" s="9" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="F136" s="9">
         <v>2011</v>
       </c>
       <c r="G136" s="13" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="H136" s="19" t="s">
         <v>229</v>
@@ -34094,23 +34097,23 @@
         <v>135</v>
       </c>
       <c r="B137" s="9" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C137" s="9" t="s">
         <v>1215</v>
-      </c>
-      <c r="C137" s="9" t="s">
-        <v>1216</v>
       </c>
       <c r="D137" s="9" t="str">
         <f t="shared" si="3"/>
         <v>stan modeling language user’s guide and reference manual</v>
       </c>
       <c r="E137" s="9" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="F137" s="9">
         <v>2016</v>
       </c>
       <c r="G137" s="13" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="H137" s="19" t="s">
         <v>229</v>
@@ -34158,10 +34161,10 @@
         <v>136</v>
       </c>
       <c r="B138" s="9" t="s">
+        <v>1218</v>
+      </c>
+      <c r="C138" s="9" t="s">
         <v>1219</v>
-      </c>
-      <c r="C138" s="9" t="s">
-        <v>1220</v>
       </c>
       <c r="D138" s="9" t="str">
         <f t="shared" si="3"/>
@@ -34171,7 +34174,7 @@
         <v>2016</v>
       </c>
       <c r="G138" s="13" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="H138" s="19" t="s">
         <v>229</v>
@@ -34219,10 +34222,10 @@
         <v>137</v>
       </c>
       <c r="B139" s="9" t="s">
+        <v>1221</v>
+      </c>
+      <c r="C139" s="9" t="s">
         <v>1222</v>
-      </c>
-      <c r="C139" s="9" t="s">
-        <v>1223</v>
       </c>
       <c r="D139" s="9" t="str">
         <f t="shared" si="3"/>
@@ -34232,7 +34235,7 @@
         <v>2016</v>
       </c>
       <c r="G139" s="13" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="H139" s="19" t="s">
         <v>229</v>
@@ -34280,10 +34283,10 @@
         <v>138</v>
       </c>
       <c r="B140" s="9" t="s">
+        <v>1224</v>
+      </c>
+      <c r="C140" s="9" t="s">
         <v>1225</v>
-      </c>
-      <c r="C140" s="9" t="s">
-        <v>1226</v>
       </c>
       <c r="D140" s="20" t="str">
         <f t="shared" si="3"/>
@@ -34296,7 +34299,7 @@
         <v>2004</v>
       </c>
       <c r="G140" s="13" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="H140" s="20" t="s">
         <v>229</v>
@@ -34344,23 +34347,23 @@
         <v>139</v>
       </c>
       <c r="B141" s="9" t="s">
+        <v>1227</v>
+      </c>
+      <c r="C141" s="20" t="s">
         <v>1228</v>
-      </c>
-      <c r="C141" s="20" t="s">
-        <v>1229</v>
       </c>
       <c r="D141" s="20" t="str">
         <f t="shared" ref="D141:D205" si="4">TRIM(LOWER(C141))</f>
         <v>extendable physical unit checking with understandable error reporting</v>
       </c>
       <c r="E141" s="9" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="F141" s="9">
         <v>2009</v>
       </c>
       <c r="G141" s="13" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="H141" s="20" t="s">
         <v>229</v>
@@ -34408,7 +34411,7 @@
         <v>140</v>
       </c>
       <c r="B142" s="9" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="C142" s="9" t="s">
         <v>914</v>
@@ -34439,10 +34442,10 @@
         <v>141</v>
       </c>
       <c r="B143" s="9" t="s">
+        <v>1232</v>
+      </c>
+      <c r="C143" s="9" t="s">
         <v>1233</v>
-      </c>
-      <c r="C143" s="9" t="s">
-        <v>1234</v>
       </c>
       <c r="D143" s="20" t="str">
         <f t="shared" si="4"/>
@@ -34452,7 +34455,7 @@
         <v>2016</v>
       </c>
       <c r="G143" s="13" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="H143" s="20" t="s">
         <v>229</v>
@@ -34500,23 +34503,23 @@
         <v>142</v>
       </c>
       <c r="B144" s="9" t="s">
+        <v>1235</v>
+      </c>
+      <c r="C144" s="9" t="s">
         <v>1236</v>
-      </c>
-      <c r="C144" s="9" t="s">
-        <v>1237</v>
       </c>
       <c r="D144" s="20" t="str">
         <f t="shared" si="4"/>
         <v>natural unit representation in modelica</v>
       </c>
       <c r="E144" s="9" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="F144" s="9">
         <v>2012</v>
       </c>
       <c r="G144" s="13" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="H144" s="20" t="s">
         <v>229</v>
@@ -34564,10 +34567,10 @@
         <v>143</v>
       </c>
       <c r="B145" s="9" t="s">
+        <v>1238</v>
+      </c>
+      <c r="C145" s="9" t="s">
         <v>1239</v>
-      </c>
-      <c r="C145" s="9" t="s">
-        <v>1240</v>
       </c>
       <c r="D145" s="20" t="str">
         <f t="shared" si="4"/>
@@ -34580,7 +34583,7 @@
         <v>2009</v>
       </c>
       <c r="G145" s="13" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
       <c r="H145" s="20" t="s">
         <v>229</v>
@@ -34631,14 +34634,14 @@
         <v>684</v>
       </c>
       <c r="C146" s="9" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="D146" s="20" t="str">
         <f t="shared" si="4"/>
         <v>quantity: represent dimensioned values with both their amount and their unit</v>
       </c>
       <c r="G146" s="13" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="H146" s="20" t="s">
         <v>229</v>
@@ -34668,7 +34671,7 @@
         <v>684</v>
       </c>
       <c r="C147" s="9" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="D147" s="20" t="str">
         <f t="shared" si="4"/>
@@ -34678,7 +34681,7 @@
         <v>1997</v>
       </c>
       <c r="G147" s="13" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="H147" s="20" t="s">
         <v>229</v>
@@ -34726,10 +34729,10 @@
         <v>146</v>
       </c>
       <c r="B148" s="9" t="s">
+        <v>1245</v>
+      </c>
+      <c r="C148" s="9" t="s">
         <v>1246</v>
-      </c>
-      <c r="C148" s="9" t="s">
-        <v>1247</v>
       </c>
       <c r="D148" s="20" t="str">
         <f t="shared" si="4"/>
@@ -34742,7 +34745,7 @@
         <v>1998</v>
       </c>
       <c r="G148" s="13" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="H148" s="20" t="s">
         <v>229</v>
@@ -34790,7 +34793,7 @@
         <v>147</v>
       </c>
       <c r="B149" s="9" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="C149" s="9" t="s">
         <v>929</v>
@@ -34821,10 +34824,10 @@
         <v>148</v>
       </c>
       <c r="B150" s="9" t="s">
+        <v>1249</v>
+      </c>
+      <c r="C150" s="9" t="s">
         <v>1250</v>
-      </c>
-      <c r="C150" s="9" t="s">
-        <v>1251</v>
       </c>
       <c r="D150" s="20" t="str">
         <f t="shared" si="4"/>
@@ -34834,7 +34837,7 @@
         <v>2016</v>
       </c>
       <c r="G150" s="13" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="H150" s="20" t="s">
         <v>229</v>
@@ -34882,10 +34885,10 @@
         <v>149</v>
       </c>
       <c r="B151" s="9" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C151" s="9" t="s">
         <v>1253</v>
-      </c>
-      <c r="C151" s="9" t="s">
-        <v>1254</v>
       </c>
       <c r="D151" s="20" t="str">
         <f t="shared" si="4"/>
@@ -34895,7 +34898,7 @@
         <v>2014</v>
       </c>
       <c r="G151" s="13" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="H151" s="20" t="s">
         <v>229</v>
@@ -34943,23 +34946,23 @@
         <v>150</v>
       </c>
       <c r="B152" s="9" t="s">
+        <v>1255</v>
+      </c>
+      <c r="C152" s="9" t="s">
         <v>1256</v>
-      </c>
-      <c r="C152" s="9" t="s">
-        <v>1257</v>
       </c>
       <c r="D152" s="20" t="str">
         <f t="shared" si="4"/>
         <v>the systems biology markup language (sbml): a medium for representation and exchange of bio- chemical network models</v>
       </c>
       <c r="E152" s="9" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="F152" s="9">
         <v>2003</v>
       </c>
       <c r="G152" s="13" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="H152" s="20" t="s">
         <v>229</v>
@@ -35007,23 +35010,23 @@
         <v>151</v>
       </c>
       <c r="B153" s="9" t="s">
+        <v>1259</v>
+      </c>
+      <c r="C153" s="9" t="s">
         <v>1260</v>
-      </c>
-      <c r="C153" s="9" t="s">
-        <v>1261</v>
       </c>
       <c r="D153" s="20" t="str">
         <f t="shared" si="4"/>
         <v>mars climate orbiter fail- ure board releases report, numerous nasa actions un- derway in response</v>
       </c>
       <c r="E153" s="9" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="F153" s="9">
         <v>1999</v>
       </c>
       <c r="G153" s="13" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="H153" s="20" t="s">
         <v>229</v>
@@ -35139,10 +35142,10 @@
         <v>154</v>
       </c>
       <c r="B156" s="9" t="s">
+        <v>1263</v>
+      </c>
+      <c r="C156" s="9" t="s">
         <v>1264</v>
-      </c>
-      <c r="C156" s="9" t="s">
-        <v>1265</v>
       </c>
       <c r="D156" s="20" t="str">
         <f t="shared" si="4"/>
@@ -35173,7 +35176,7 @@
         <v>155</v>
       </c>
       <c r="B157" s="9" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="C157" s="9" t="s">
         <v>946</v>
@@ -35183,7 +35186,7 @@
         <v>generating optimized configurable business process models in scenarios subject to uncertainty</v>
       </c>
       <c r="E157" s="9" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="H157" s="20" t="s">
         <v>229</v>
@@ -35207,10 +35210,10 @@
         <v>156</v>
       </c>
       <c r="B158" s="9" t="s">
+        <v>1267</v>
+      </c>
+      <c r="C158" s="9" t="s">
         <v>1268</v>
-      </c>
-      <c r="C158" s="9" t="s">
-        <v>1269</v>
       </c>
       <c r="D158" s="20" t="str">
         <f t="shared" si="4"/>
@@ -35220,7 +35223,7 @@
         <v>2002</v>
       </c>
       <c r="G158" s="13" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="H158" s="20" t="s">
         <v>229</v>
@@ -35268,10 +35271,10 @@
         <v>157</v>
       </c>
       <c r="B159" s="9" t="s">
+        <v>1270</v>
+      </c>
+      <c r="C159" s="9" t="s">
         <v>1271</v>
-      </c>
-      <c r="C159" s="9" t="s">
-        <v>1272</v>
       </c>
       <c r="D159" s="20" t="str">
         <f t="shared" si="4"/>
@@ -35284,7 +35287,7 @@
         <v>1997</v>
       </c>
       <c r="G159" s="13" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="H159" s="20" t="s">
         <v>229</v>
@@ -35332,23 +35335,23 @@
         <v>158</v>
       </c>
       <c r="B160" s="9" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="C160" s="20" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="D160" s="20" t="str">
         <f t="shared" si="4"/>
         <v>types for units-of-measure: theory and practice</v>
       </c>
       <c r="E160" s="9" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="F160" s="9">
         <v>2009</v>
       </c>
       <c r="G160" s="13" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="H160" s="20" t="s">
         <v>229</v>
@@ -35396,10 +35399,10 @@
         <v>159</v>
       </c>
       <c r="B161" s="9" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C161" s="9" t="s">
         <v>1277</v>
-      </c>
-      <c r="C161" s="9" t="s">
-        <v>1278</v>
       </c>
       <c r="D161" s="20" t="str">
         <f t="shared" si="4"/>
@@ -35409,7 +35412,7 @@
         <v>2016</v>
       </c>
       <c r="G161" s="13" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="H161" s="20" t="s">
         <v>229</v>
@@ -35457,7 +35460,7 @@
         <v>160</v>
       </c>
       <c r="B162" s="9" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="C162" s="9" t="s">
         <v>954</v>
@@ -35491,10 +35494,10 @@
         <v>161</v>
       </c>
       <c r="B163" s="9" t="s">
+        <v>1280</v>
+      </c>
+      <c r="C163" s="9" t="s">
         <v>1281</v>
-      </c>
-      <c r="C163" s="9" t="s">
-        <v>1282</v>
       </c>
       <c r="D163" s="20" t="str">
         <f t="shared" si="4"/>
@@ -35504,7 +35507,7 @@
         <v>2016</v>
       </c>
       <c r="G163" s="13" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="H163" s="20" t="s">
         <v>229</v>
@@ -35552,23 +35555,23 @@
         <v>162</v>
       </c>
       <c r="B164" s="9" t="s">
+        <v>1283</v>
+      </c>
+      <c r="C164" s="9" t="s">
         <v>1284</v>
-      </c>
-      <c r="C164" s="9" t="s">
-        <v>1285</v>
       </c>
       <c r="D164" s="20" t="str">
         <f t="shared" si="4"/>
         <v>unit checking and quantity conservation</v>
       </c>
       <c r="E164" s="9" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="F164" s="9">
         <v>2008</v>
       </c>
       <c r="G164" s="13" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="H164" s="20" t="s">
         <v>229</v>
@@ -35616,10 +35619,10 @@
         <v>163</v>
       </c>
       <c r="B165" s="9" t="s">
+        <v>1286</v>
+      </c>
+      <c r="C165" s="9" t="s">
         <v>1287</v>
-      </c>
-      <c r="C165" s="9" t="s">
-        <v>1288</v>
       </c>
       <c r="D165" s="20" t="str">
         <f t="shared" si="4"/>
@@ -35632,7 +35635,7 @@
         <v>2013</v>
       </c>
       <c r="G165" s="13" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="H165" s="20" t="s">
         <v>229</v>
@@ -35680,10 +35683,10 @@
         <v>164</v>
       </c>
       <c r="B166" s="9" t="s">
+        <v>1289</v>
+      </c>
+      <c r="C166" s="9" t="s">
         <v>1290</v>
-      </c>
-      <c r="C166" s="9" t="s">
-        <v>1291</v>
       </c>
       <c r="D166" s="20" t="str">
         <f t="shared" si="4"/>
@@ -35693,7 +35696,7 @@
         <v>2016</v>
       </c>
       <c r="G166" s="13" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="H166" s="20" t="s">
         <v>229</v>
@@ -35741,10 +35744,10 @@
         <v>165</v>
       </c>
       <c r="B167" s="9" t="s">
+        <v>1292</v>
+      </c>
+      <c r="C167" s="9" t="s">
         <v>1293</v>
-      </c>
-      <c r="C167" s="9" t="s">
-        <v>1294</v>
       </c>
       <c r="D167" s="20" t="str">
         <f t="shared" si="4"/>
@@ -35757,7 +35760,7 @@
         <v>2016</v>
       </c>
       <c r="G167" s="13" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="H167" s="20" t="s">
         <v>229</v>
@@ -35932,7 +35935,7 @@
         <v>968</v>
       </c>
       <c r="C172" s="9" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="D172" s="20" t="str">
         <f t="shared" si="4"/>
@@ -35945,7 +35948,7 @@
         <v>2016</v>
       </c>
       <c r="G172" s="13" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="H172" s="20" t="s">
         <v>229</v>
@@ -35993,10 +35996,10 @@
         <v>171</v>
       </c>
       <c r="B173" s="9" t="s">
+        <v>1297</v>
+      </c>
+      <c r="C173" s="9" t="s">
         <v>1298</v>
-      </c>
-      <c r="C173" s="9" t="s">
-        <v>1299</v>
       </c>
       <c r="D173" s="20" t="str">
         <f t="shared" si="4"/>
@@ -36006,7 +36009,7 @@
         <v>2016</v>
       </c>
       <c r="G173" s="13" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="H173" s="20" t="s">
         <v>229</v>
@@ -36054,23 +36057,23 @@
         <v>172</v>
       </c>
       <c r="B174" s="9" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C174" s="9" t="s">
         <v>1301</v>
-      </c>
-      <c r="C174" s="9" t="s">
-        <v>1302</v>
       </c>
       <c r="D174" s="20" t="str">
         <f t="shared" si="4"/>
         <v>cyber- physical systems: the next computing revolution</v>
       </c>
       <c r="E174" s="9" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F174" s="9">
         <v>2010</v>
       </c>
       <c r="G174" s="13" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="H174" s="20" t="s">
         <v>229</v>
@@ -36118,10 +36121,10 @@
         <v>173</v>
       </c>
       <c r="B175" s="9" t="s">
+        <v>1304</v>
+      </c>
+      <c r="C175" s="9" t="s">
         <v>1305</v>
-      </c>
-      <c r="C175" s="9" t="s">
-        <v>1306</v>
       </c>
       <c r="D175" s="20" t="str">
         <f t="shared" si="4"/>
@@ -36131,7 +36134,7 @@
         <v>2007</v>
       </c>
       <c r="G175" s="13" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="H175" s="20" t="s">
         <v>229</v>
@@ -36179,7 +36182,7 @@
         <v>174</v>
       </c>
       <c r="B176" s="9" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="C176" s="9" t="s">
         <v>984</v>
@@ -36210,23 +36213,23 @@
         <v>175</v>
       </c>
       <c r="B177" s="9" t="s">
+        <v>1308</v>
+      </c>
+      <c r="C177" s="9" t="s">
         <v>1309</v>
-      </c>
-      <c r="C177" s="9" t="s">
-        <v>1310</v>
       </c>
       <c r="D177" s="20" t="str">
         <f t="shared" si="4"/>
         <v>the international system of units (si)</v>
       </c>
       <c r="E177" s="9" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="F177" s="9">
         <v>2008</v>
       </c>
       <c r="G177" s="13" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="H177" s="20" t="s">
         <v>229</v>
@@ -36274,7 +36277,7 @@
         <v>176</v>
       </c>
       <c r="B178" s="9" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="C178" s="22" t="s">
         <v>876</v>
@@ -36305,7 +36308,7 @@
         <v>177</v>
       </c>
       <c r="B179" s="9" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="C179" s="9" t="s">
         <v>992</v>
@@ -36336,10 +36339,10 @@
         <v>178</v>
       </c>
       <c r="B180" s="9" t="s">
+        <v>1314</v>
+      </c>
+      <c r="C180" s="20" t="s">
         <v>1315</v>
-      </c>
-      <c r="C180" s="20" t="s">
-        <v>1316</v>
       </c>
       <c r="D180" s="20" t="str">
         <f t="shared" si="4"/>
@@ -36349,7 +36352,7 @@
         <v>2016</v>
       </c>
       <c r="G180" s="13" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="H180" s="20" t="s">
         <v>229</v>
@@ -36397,7 +36400,7 @@
         <v>179</v>
       </c>
       <c r="B181" s="9" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="C181" s="9" t="s">
         <v>954</v>
@@ -36428,7 +36431,7 @@
         <v>180</v>
       </c>
       <c r="B182" s="9" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="C182" s="9" t="s">
         <v>910</v>
@@ -36459,7 +36462,7 @@
         <v>181</v>
       </c>
       <c r="B183" s="9" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="C183" s="9" t="s">
         <v>984</v>
@@ -36490,10 +36493,10 @@
         <v>182</v>
       </c>
       <c r="B184" s="9" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="C184" s="9" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="D184" s="21" t="str">
         <f t="shared" si="4"/>
@@ -36506,7 +36509,7 @@
         <v>2016</v>
       </c>
       <c r="G184" s="13" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="H184" s="21" t="s">
         <v>229</v>
@@ -36622,10 +36625,10 @@
         <v>185</v>
       </c>
       <c r="B187" s="9" t="s">
+        <v>1263</v>
+      </c>
+      <c r="C187" s="9" t="s">
         <v>1264</v>
-      </c>
-      <c r="C187" s="9" t="s">
-        <v>1265</v>
       </c>
       <c r="D187" s="21" t="str">
         <f t="shared" si="4"/>
@@ -36724,7 +36727,7 @@
         <v>188</v>
       </c>
       <c r="B190" s="21" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="C190" s="9" t="s">
         <v>946</v>
@@ -36734,7 +36737,7 @@
         <v>generating optimized configurable business process models in scenarios subject to uncertainty</v>
       </c>
       <c r="E190" s="9" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="H190" s="21" t="s">
         <v>229</v>
@@ -36851,10 +36854,10 @@
         <v>192</v>
       </c>
       <c r="B194" s="9" t="s">
+        <v>1321</v>
+      </c>
+      <c r="C194" s="9" t="s">
         <v>1322</v>
-      </c>
-      <c r="C194" s="9" t="s">
-        <v>1323</v>
       </c>
       <c r="D194" s="21" t="str">
         <f t="shared" si="4"/>
@@ -36867,7 +36870,7 @@
         <v>2008</v>
       </c>
       <c r="G194" s="13" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="H194" s="21" t="s">
         <v>229</v>
@@ -36915,23 +36918,23 @@
         <v>193</v>
       </c>
       <c r="B195" s="9" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="C195" s="9" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="D195" s="21" t="str">
         <f t="shared" si="4"/>
         <v>specifying aggregation functions in multidimensional models with ocl</v>
       </c>
       <c r="E195" s="9" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="F195" s="9">
         <v>2010</v>
       </c>
       <c r="G195" s="13" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="H195" s="21" t="s">
         <v>229</v>
@@ -36979,23 +36982,23 @@
         <v>194</v>
       </c>
       <c r="B196" s="9" t="s">
+        <v>1328</v>
+      </c>
+      <c r="C196" s="9" t="s">
         <v>1329</v>
-      </c>
-      <c r="C196" s="9" t="s">
-        <v>1330</v>
       </c>
       <c r="D196" s="21" t="str">
         <f t="shared" si="4"/>
         <v>benefits and problems of formal methods</v>
       </c>
       <c r="E196" s="9" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="F196" s="9">
         <v>2004</v>
       </c>
       <c r="G196" s="13" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
       <c r="H196" s="21" t="s">
         <v>229</v>
@@ -37043,23 +37046,23 @@
         <v>195</v>
       </c>
       <c r="B197" s="9" t="s">
+        <v>1331</v>
+      </c>
+      <c r="C197" s="9" t="s">
         <v>1332</v>
-      </c>
-      <c r="C197" s="9" t="s">
-        <v>1333</v>
       </c>
       <c r="D197" s="21" t="str">
         <f t="shared" si="4"/>
         <v>a summary of error propagation</v>
       </c>
       <c r="E197" s="9" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="F197" s="9">
         <v>2014</v>
       </c>
       <c r="G197" s="13" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="H197" s="21" t="s">
         <v>229</v>
@@ -37107,10 +37110,10 @@
         <v>196</v>
       </c>
       <c r="B198" s="9" t="s">
+        <v>1335</v>
+      </c>
+      <c r="C198" s="9" t="s">
         <v>1336</v>
-      </c>
-      <c r="C198" s="9" t="s">
-        <v>1337</v>
       </c>
       <c r="D198" s="21" t="str">
         <f t="shared" si="4"/>
@@ -37120,7 +37123,7 @@
         <v>2015</v>
       </c>
       <c r="G198" s="13" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="H198" s="21" t="s">
         <v>229</v>
@@ -37168,10 +37171,10 @@
         <v>197</v>
       </c>
       <c r="B199" s="9" t="s">
+        <v>1292</v>
+      </c>
+      <c r="C199" s="9" t="s">
         <v>1293</v>
-      </c>
-      <c r="C199" s="9" t="s">
-        <v>1294</v>
       </c>
       <c r="D199" s="21" t="str">
         <f t="shared" si="4"/>
@@ -37199,23 +37202,23 @@
         <v>198</v>
       </c>
       <c r="B200" s="9" t="s">
+        <v>1338</v>
+      </c>
+      <c r="C200" s="9" t="s">
         <v>1339</v>
-      </c>
-      <c r="C200" s="9" t="s">
-        <v>1340</v>
       </c>
       <c r="D200" s="21" t="str">
         <f t="shared" si="4"/>
         <v>accuracy and stability of numerical algorithms</v>
       </c>
       <c r="E200" s="9" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="F200" s="9">
         <v>1996</v>
       </c>
       <c r="G200" s="13" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="H200" s="21" t="s">
         <v>229</v>
@@ -37263,23 +37266,23 @@
         <v>199</v>
       </c>
       <c r="B201" s="9" t="s">
+        <v>1342</v>
+      </c>
+      <c r="C201" s="22" t="s">
         <v>1343</v>
-      </c>
-      <c r="C201" s="22" t="s">
-        <v>1344</v>
       </c>
       <c r="D201" s="21" t="str">
         <f t="shared" si="4"/>
         <v>handbook of floating-point arithmetic</v>
       </c>
       <c r="E201" s="9" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="F201" s="9">
         <v>2010</v>
       </c>
       <c r="G201" s="13" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="H201" s="21" t="s">
         <v>229</v>
@@ -37327,23 +37330,23 @@
         <v>200</v>
       </c>
       <c r="B202" s="9" t="s">
+        <v>1346</v>
+      </c>
+      <c r="C202" s="9" t="s">
         <v>1347</v>
-      </c>
-      <c r="C202" s="9" t="s">
-        <v>1348</v>
       </c>
       <c r="D202" s="21" t="str">
         <f t="shared" si="4"/>
         <v>the guesstimate blog</v>
       </c>
       <c r="E202" s="9" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="F202" s="9">
         <v>2015</v>
       </c>
       <c r="G202" s="13" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="H202" s="21" t="s">
         <v>229</v>
@@ -37391,10 +37394,10 @@
         <v>201</v>
       </c>
       <c r="B203" s="9" t="s">
+        <v>1350</v>
+      </c>
+      <c r="C203" s="9" t="s">
         <v>1351</v>
-      </c>
-      <c r="C203" s="9" t="s">
-        <v>1352</v>
       </c>
       <c r="D203" s="21" t="str">
         <f t="shared" si="4"/>
@@ -37455,7 +37458,7 @@
         <v>202</v>
       </c>
       <c r="B204" s="9" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="C204" s="9" t="s">
         <v>925</v>
@@ -37486,7 +37489,7 @@
         <v>203</v>
       </c>
       <c r="B205" s="9" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="C205" s="9" t="s">
         <v>797</v>
@@ -37517,7 +37520,7 @@
         <v>204</v>
       </c>
       <c r="B206" s="9" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="C206" s="9" t="s">
         <v>921</v>
@@ -37548,7 +37551,7 @@
         <v>205</v>
       </c>
       <c r="B207" s="9" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="C207" s="9" t="s">
         <v>981</v>
@@ -37579,10 +37582,10 @@
         <v>206</v>
       </c>
       <c r="B208" s="9" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="C208" s="9" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="D208" s="21" t="str">
         <f t="shared" si="6"/>
@@ -37610,7 +37613,7 @@
         <v>207</v>
       </c>
       <c r="B209" s="9" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="C209" s="9" t="s">
         <v>936</v>
@@ -37641,7 +37644,7 @@
         <v>208</v>
       </c>
       <c r="B210" s="9" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="C210" s="9" t="s">
         <v>929</v>
@@ -37675,7 +37678,7 @@
         <v>968</v>
       </c>
       <c r="C211" s="9" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="D211" s="21" t="str">
         <f t="shared" si="6"/>
@@ -37703,10 +37706,10 @@
         <v>210</v>
       </c>
       <c r="B212" s="9" t="s">
+        <v>1286</v>
+      </c>
+      <c r="C212" s="9" t="s">
         <v>1287</v>
-      </c>
-      <c r="C212" s="9" t="s">
-        <v>1288</v>
       </c>
       <c r="D212" s="21" t="str">
         <f t="shared" si="6"/>

</xml_diff>